<commit_message>
updating CoreMethords,Excel read, static entry
</commit_message>
<xml_diff>
--- a/myprojects/src/test/java/TestDataRepository/TestData.xlsx
+++ b/myprojects/src/test/java/TestDataRepository/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332127F4-D3ED-46C0-80F7-1CA7DF1168DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Attributes</t>
   </si>
@@ -39,9 +40,6 @@
     <t>CustomerDateOfBirth</t>
   </si>
   <si>
-    <t>15-05-1991</t>
-  </si>
-  <si>
     <t>CustomerAddress</t>
   </si>
   <si>
@@ -72,23 +70,20 @@
     <t>9584249412</t>
   </si>
   <si>
-    <t>CustomerEmailId</t>
-  </si>
-  <si>
     <t>CustomerPassword</t>
   </si>
   <si>
     <t>qwerty123</t>
   </si>
   <si>
-    <t>y1233@ybtgdgc.com</t>
+    <t>05051991</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +121,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -172,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +207,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,6 +259,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,16 +452,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -438,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -446,97 +489,86 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="y1@ydddfbc.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Balance enquiry, mini statement,delete account and customised statement
</commit_message>
<xml_diff>
--- a/myprojects/src/test/java/TestDataRepository/TestData.xlsx
+++ b/myprojects/src/test/java/TestDataRepository/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE51A5E2-EFDF-4359-99D8-D0B46D968F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158E0203-2013-4831-A276-3F9FA38DA5A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Attributes</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>87270</t>
+  </si>
+  <si>
+    <t>AccountIDForDelete</t>
+  </si>
+  <si>
+    <t>78178</t>
   </si>
 </sst>
 </file>
@@ -130,10 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,6 +593,14 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>